<commit_message>
Additional translations and corrections in management files
</commit_message>
<xml_diff>
--- a/data/management/Management_information_QLB_2015.xlsx
+++ b/data/management/Management_information_QLB_2015.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillrose/Library/Mobile Documents/com~apple~CloudDocs/iCloud Daten/Arbeit/R-Projects/Git_Repositories/BRIWECS_Data_Publication_2/data/management/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FED71-70A0-384A-81FF-1714D6DCAD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="23250" windowHeight="13170"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="37480" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
   <si>
     <t>06484</t>
   </si>
@@ -313,12 +319,6 @@
   </si>
   <si>
     <t>Prosaro</t>
-  </si>
-  <si>
-    <t>50 kg N/ha</t>
-  </si>
-  <si>
-    <t>40 kg N/ha</t>
   </si>
   <si>
     <t>CAN</t>
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,7 +597,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
@@ -625,10 +625,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -655,10 +651,10 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20 % - Akzent3" xfId="3" builtinId="38"/>
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
-    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -666,14 +662,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -711,7 +710,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -783,7 +782,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -956,32 +955,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P92" sqref="P92"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="10" max="15" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="28.5703125" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="10" max="15" width="16.83203125" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -989,15 +988,15 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1005,23 +1004,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1029,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1053,13 +1052,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1083,7 +1082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1091,140 +1090,140 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>107</v>
+      <c r="B21" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="13">
         <v>95</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>108</v>
+      <c r="B23" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>109</v>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>110</v>
+      <c r="B25" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>111</v>
+      <c r="B26" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>112</v>
+      <c r="B27" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>126</v>
+      <c r="B29" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>126</v>
+      <c r="B30" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>126</v>
+      <c r="B31" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="13">
         <v>6.8</v>
       </c>
       <c r="C32" s="11">
         <v>41889</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>41889</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -1257,14 +1256,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>64</v>
       </c>
@@ -1286,7 +1285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
@@ -1319,8 +1318,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>81</v>
       </c>
@@ -1341,7 +1340,7 @@
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
     </row>
-    <row r="44" spans="1:17" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>68</v>
       </c>
@@ -1373,28 +1372,28 @@
         <v>70</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L44" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="M44" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N44" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="M44" s="10" t="s">
+      <c r="O44" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="N44" s="10" t="s">
+      <c r="P44" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="O44" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="P44" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="Q44" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1419,29 +1418,29 @@
       <c r="J45" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K45" s="23">
+      <c r="K45" s="21">
         <v>42102</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="21">
         <v>42114</v>
       </c>
-      <c r="M45" s="23">
+      <c r="M45" s="21">
         <v>42135</v>
       </c>
-      <c r="N45" s="23">
+      <c r="N45" s="21">
         <v>42150</v>
       </c>
-      <c r="O45" s="23">
+      <c r="O45" s="21">
         <v>42165</v>
       </c>
-      <c r="P45" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q45" s="26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P45" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q45" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -1461,26 +1460,26 @@
         <v>72</v>
       </c>
       <c r="K46" s="8"/>
-      <c r="L46" s="23">
+      <c r="L46" s="21">
         <v>42114</v>
       </c>
-      <c r="M46" s="23">
+      <c r="M46" s="21">
         <v>42135</v>
       </c>
-      <c r="N46" s="23">
+      <c r="N46" s="21">
         <v>42171</v>
       </c>
-      <c r="O46" s="23">
+      <c r="O46" s="21">
         <v>42185</v>
       </c>
-      <c r="P46" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q46" s="27">
+      <c r="P46" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q46" s="25">
         <v>42215</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -1505,23 +1504,23 @@
       <c r="J47" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K47" s="23">
+      <c r="K47" s="21">
         <v>42145</v>
       </c>
-      <c r="L47" s="23">
+      <c r="L47" s="21">
         <v>42152</v>
       </c>
-      <c r="M47" s="23">
+      <c r="M47" s="21">
         <v>42171</v>
       </c>
-      <c r="N47" s="23">
+      <c r="N47" s="21">
         <v>42185</v>
       </c>
-      <c r="O47" s="24"/>
-      <c r="P47" s="28"/>
-      <c r="Q47" s="28"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O47" s="22"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>69</v>
       </c>
@@ -1541,16 +1540,16 @@
         <v>74</v>
       </c>
       <c r="K48" s="8"/>
-      <c r="L48" s="23">
+      <c r="L48" s="21">
         <v>42114</v>
       </c>
-      <c r="M48" s="24"/>
-      <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="28"/>
-      <c r="Q48" s="28"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M48" s="22"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="26"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -1568,14 +1567,14 @@
         <v>75</v>
       </c>
       <c r="K49" s="8"/>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="24"/>
-      <c r="P49" s="28"/>
-      <c r="Q49" s="28"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="26"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -1593,20 +1592,20 @@
         <v>76</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="L50" s="23">
+        <v>101</v>
+      </c>
+      <c r="L50" s="21">
         <v>42185</v>
       </c>
-      <c r="M50" s="23">
+      <c r="M50" s="21">
         <v>42192</v>
       </c>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
-      <c r="P50" s="28"/>
-      <c r="Q50" s="28"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="26"/>
+      <c r="Q50" s="26"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>69</v>
       </c>
@@ -1622,14 +1621,14 @@
       <c r="I51" s="7"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="28"/>
-      <c r="Q51" s="28"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="26"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -1651,14 +1650,14 @@
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="28"/>
-      <c r="Q52" s="28"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="26"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -1680,20 +1679,20 @@
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="24"/>
-      <c r="O53" s="24"/>
-      <c r="P53" s="28"/>
-      <c r="Q53" s="28"/>
-    </row>
-    <row r="54" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-    </row>
-    <row r="55" spans="1:17" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="26"/>
+    </row>
+    <row r="54" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+    </row>
+    <row r="55" spans="1:17" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>68</v>
       </c>
@@ -1725,28 +1724,28 @@
         <v>70</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="L55" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="L55" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M55" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="N55" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="M55" s="21" t="s">
+      <c r="O55" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="N55" s="21" t="s">
+      <c r="P55" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="O55" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="P55" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="Q55" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -1772,18 +1771,18 @@
         <v>71</v>
       </c>
       <c r="K56" s="8"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="24"/>
-      <c r="N56" s="24"/>
-      <c r="O56" s="24"/>
-      <c r="P56" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q56" s="26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q56" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -1803,18 +1802,18 @@
         <v>72</v>
       </c>
       <c r="K57" s="8"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="24"/>
-      <c r="O57" s="24"/>
-      <c r="P57" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q57" s="27">
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q57" s="25">
         <v>42215</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -1840,14 +1839,14 @@
         <v>73</v>
       </c>
       <c r="K58" s="8"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="24"/>
-      <c r="N58" s="24"/>
-      <c r="O58" s="24"/>
-      <c r="P58" s="28"/>
-      <c r="Q58" s="28"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="26"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -1867,14 +1866,14 @@
         <v>74</v>
       </c>
       <c r="K59" s="8"/>
-      <c r="L59" s="24"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="24"/>
-      <c r="O59" s="24"/>
-      <c r="P59" s="28"/>
-      <c r="Q59" s="28"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="26"/>
+      <c r="Q59" s="26"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -1898,14 +1897,14 @@
         <v>75</v>
       </c>
       <c r="K60" s="8"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="24"/>
-      <c r="O60" s="24"/>
-      <c r="P60" s="28"/>
-      <c r="Q60" s="28"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="26"/>
+      <c r="Q60" s="26"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -1929,14 +1928,14 @@
         <v>76</v>
       </c>
       <c r="K61" s="8"/>
-      <c r="L61" s="24"/>
-      <c r="M61" s="24"/>
-      <c r="N61" s="24"/>
-      <c r="O61" s="24"/>
-      <c r="P61" s="28"/>
-      <c r="Q61" s="28"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="26"/>
+      <c r="Q61" s="26"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -1958,14 +1957,14 @@
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
-      <c r="L62" s="24"/>
-      <c r="M62" s="24"/>
-      <c r="N62" s="24"/>
-      <c r="O62" s="24"/>
-      <c r="P62" s="28"/>
-      <c r="Q62" s="28"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="22"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="26"/>
+      <c r="Q62" s="26"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -1987,14 +1986,14 @@
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
-      <c r="L63" s="24"/>
-      <c r="M63" s="24"/>
-      <c r="N63" s="24"/>
-      <c r="O63" s="24"/>
-      <c r="P63" s="28"/>
-      <c r="Q63" s="28"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="26"/>
+      <c r="Q63" s="26"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2016,20 +2015,20 @@
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
-      <c r="L64" s="24"/>
-      <c r="M64" s="24"/>
-      <c r="N64" s="24"/>
-      <c r="O64" s="24"/>
-      <c r="P64" s="28"/>
-      <c r="Q64" s="28"/>
-    </row>
-    <row r="65" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L65" s="19"/>
-      <c r="M65" s="19"/>
-      <c r="N65" s="19"/>
-      <c r="O65" s="19"/>
-    </row>
-    <row r="66" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
+      <c r="P64" s="26"/>
+      <c r="Q64" s="26"/>
+    </row>
+    <row r="65" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+    </row>
+    <row r="66" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>68</v>
       </c>
@@ -2061,28 +2060,28 @@
         <v>70</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="L66" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="L66" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="N66" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="M66" s="21" t="s">
+      <c r="O66" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="N66" s="21" t="s">
+      <c r="P66" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="O66" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="P66" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="Q66" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -2092,11 +2091,11 @@
       <c r="C67" s="15">
         <v>42107</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="16">
+        <v>50</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>17</v>
@@ -2113,29 +2112,29 @@
       <c r="J67" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K67" s="23">
+      <c r="K67" s="21">
         <v>42102</v>
       </c>
-      <c r="L67" s="23">
+      <c r="L67" s="21">
         <v>42114</v>
       </c>
-      <c r="M67" s="23">
+      <c r="M67" s="21">
         <v>42135</v>
       </c>
-      <c r="N67" s="23">
+      <c r="N67" s="21">
         <v>42150</v>
       </c>
-      <c r="O67" s="23">
+      <c r="O67" s="21">
         <v>42165</v>
       </c>
-      <c r="P67" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q67" s="26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P67" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q67" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -2145,11 +2144,11 @@
       <c r="C68" s="15">
         <v>42137</v>
       </c>
-      <c r="D68" s="16" t="s">
-        <v>100</v>
+      <c r="D68" s="16">
+        <v>40</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>18</v>
@@ -2161,26 +2160,26 @@
         <v>72</v>
       </c>
       <c r="K68" s="8"/>
-      <c r="L68" s="23">
+      <c r="L68" s="21">
         <v>42114</v>
       </c>
-      <c r="M68" s="23">
+      <c r="M68" s="21">
         <v>42135</v>
       </c>
-      <c r="N68" s="23">
+      <c r="N68" s="21">
         <v>42171</v>
       </c>
-      <c r="O68" s="23">
+      <c r="O68" s="21">
         <v>42185</v>
       </c>
-      <c r="P68" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q68" s="27">
+      <c r="P68" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q68" s="25">
         <v>42216</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2205,23 +2204,23 @@
       <c r="J69" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K69" s="23">
+      <c r="K69" s="21">
         <v>42145</v>
       </c>
-      <c r="L69" s="23">
+      <c r="L69" s="21">
         <v>42152</v>
       </c>
-      <c r="M69" s="23">
+      <c r="M69" s="21">
         <v>42171</v>
       </c>
-      <c r="N69" s="23">
+      <c r="N69" s="21">
         <v>42185</v>
       </c>
-      <c r="O69" s="24"/>
-      <c r="P69" s="28"/>
-      <c r="Q69" s="28"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O69" s="22"/>
+      <c r="P69" s="26"/>
+      <c r="Q69" s="26"/>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2241,16 +2240,16 @@
         <v>74</v>
       </c>
       <c r="K70" s="8"/>
-      <c r="L70" s="23">
+      <c r="L70" s="21">
         <v>42114</v>
       </c>
-      <c r="M70" s="24"/>
-      <c r="N70" s="24"/>
-      <c r="O70" s="24"/>
-      <c r="P70" s="28"/>
-      <c r="Q70" s="28"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M70" s="22"/>
+      <c r="N70" s="22"/>
+      <c r="O70" s="22"/>
+      <c r="P70" s="26"/>
+      <c r="Q70" s="26"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2268,14 +2267,14 @@
         <v>75</v>
       </c>
       <c r="K71" s="8"/>
-      <c r="L71" s="24"/>
-      <c r="M71" s="24"/>
-      <c r="N71" s="24"/>
-      <c r="O71" s="24"/>
-      <c r="P71" s="28"/>
-      <c r="Q71" s="28"/>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L71" s="22"/>
+      <c r="M71" s="22"/>
+      <c r="N71" s="22"/>
+      <c r="O71" s="22"/>
+      <c r="P71" s="26"/>
+      <c r="Q71" s="26"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -2293,20 +2292,20 @@
         <v>76</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="L72" s="23">
+        <v>101</v>
+      </c>
+      <c r="L72" s="21">
         <v>42185</v>
       </c>
-      <c r="M72" s="23">
+      <c r="M72" s="21">
         <v>42192</v>
       </c>
-      <c r="N72" s="24"/>
-      <c r="O72" s="24"/>
-      <c r="P72" s="28"/>
-      <c r="Q72" s="28"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N72" s="22"/>
+      <c r="O72" s="22"/>
+      <c r="P72" s="26"/>
+      <c r="Q72" s="26"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -2326,10 +2325,10 @@
       <c r="M73" s="8"/>
       <c r="N73" s="8"/>
       <c r="O73" s="8"/>
-      <c r="P73" s="28"/>
-      <c r="Q73" s="28"/>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P73" s="26"/>
+      <c r="Q73" s="26"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2355,10 +2354,10 @@
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
       <c r="O74" s="8"/>
-      <c r="P74" s="28"/>
-      <c r="Q74" s="28"/>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P74" s="26"/>
+      <c r="Q74" s="26"/>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -2384,11 +2383,11 @@
       <c r="M75" s="8"/>
       <c r="N75" s="8"/>
       <c r="O75" s="8"/>
-      <c r="P75" s="28"/>
-      <c r="Q75" s="28"/>
-    </row>
-    <row r="76" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:17" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P75" s="26"/>
+      <c r="Q75" s="26"/>
+    </row>
+    <row r="76" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:17" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>68</v>
       </c>
@@ -2420,28 +2419,28 @@
         <v>70</v>
       </c>
       <c r="K77" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L77" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="M77" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N77" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="M77" s="10" t="s">
+      <c r="O77" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="N77" s="10" t="s">
+      <c r="P77" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="O77" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="P77" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="Q77" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -2451,11 +2450,11 @@
       <c r="C78" s="15">
         <v>42107</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D78" s="16">
+        <v>50</v>
+      </c>
+      <c r="E78" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>17</v>
@@ -2477,14 +2476,14 @@
       <c r="M78" s="8"/>
       <c r="N78" s="8"/>
       <c r="O78" s="8"/>
-      <c r="P78" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q78" s="26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P78" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q78" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2494,11 +2493,11 @@
       <c r="C79" s="15">
         <v>42137</v>
       </c>
-      <c r="D79" s="16" t="s">
-        <v>100</v>
+      <c r="D79" s="16">
+        <v>40</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>18</v>
@@ -2514,14 +2513,14 @@
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
       <c r="O79" s="8"/>
-      <c r="P79" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q79" s="27">
+      <c r="P79" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q79" s="25">
         <v>42216</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -2551,10 +2550,10 @@
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
       <c r="O80" s="8"/>
-      <c r="P80" s="28"/>
-      <c r="Q80" s="28"/>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P80" s="26"/>
+      <c r="Q80" s="26"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -2578,10 +2577,10 @@
       <c r="M81" s="8"/>
       <c r="N81" s="8"/>
       <c r="O81" s="8"/>
-      <c r="P81" s="28"/>
-      <c r="Q81" s="28"/>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P81" s="26"/>
+      <c r="Q81" s="26"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2609,10 +2608,10 @@
       <c r="M82" s="8"/>
       <c r="N82" s="8"/>
       <c r="O82" s="8"/>
-      <c r="P82" s="28"/>
-      <c r="Q82" s="28"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P82" s="26"/>
+      <c r="Q82" s="26"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2640,10 +2639,10 @@
       <c r="M83" s="8"/>
       <c r="N83" s="8"/>
       <c r="O83" s="8"/>
-      <c r="P83" s="28"/>
-      <c r="Q83" s="28"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P83" s="26"/>
+      <c r="Q83" s="26"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -2669,10 +2668,10 @@
       <c r="M84" s="8"/>
       <c r="N84" s="8"/>
       <c r="O84" s="8"/>
-      <c r="P84" s="28"/>
-      <c r="Q84" s="28"/>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P84" s="26"/>
+      <c r="Q84" s="26"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -2698,10 +2697,10 @@
       <c r="M85" s="8"/>
       <c r="N85" s="8"/>
       <c r="O85" s="8"/>
-      <c r="P85" s="28"/>
-      <c r="Q85" s="28"/>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P85" s="26"/>
+      <c r="Q85" s="26"/>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -2727,8 +2726,8 @@
       <c r="M86" s="8"/>
       <c r="N86" s="8"/>
       <c r="O86" s="8"/>
-      <c r="P86" s="28"/>
-      <c r="Q86" s="28"/>
+      <c r="P86" s="26"/>
+      <c r="Q86" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2736,24 +2735,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>